<commit_message>
Change Name of the Code
</commit_message>
<xml_diff>
--- a/cse.xlsx
+++ b/cse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steveli/Developer/Python/ECE143_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21871892-C96E-6B45-B171-4632524A1458}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405AD80F-A32C-944F-841B-2305A014298F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="37900" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27904,16 +27904,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>252061</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>116336</xdr:colOff>
+      <xdr:row>459</xdr:row>
+      <xdr:rowOff>29084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>649541</xdr:colOff>
-      <xdr:row>487</xdr:row>
-      <xdr:rowOff>38779</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>562289</xdr:colOff>
+      <xdr:row>505</xdr:row>
+      <xdr:rowOff>9695</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28265,7 +28265,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N458"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A237" zoomScale="131" workbookViewId="0">
       <selection sqref="A1:N237"/>
     </sheetView>
   </sheetViews>

</xml_diff>